<commit_message>
Default population of student dropdown
</commit_message>
<xml_diff>
--- a/student_list.xlsx
+++ b/student_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sarfaraz\Darul-Huda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sarfaraz\Darul-Huda\git-repo\result_password\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AE3496-0B7D-4B86-95BC-6D6397E26B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A498B1-8175-4ED5-BED8-D057DB1F4243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,13 +33,13 @@
     <t>Names</t>
   </si>
   <si>
-    <t>Muhammad</t>
+    <t>GULAM GOS HABIB SHAIKH.pdf</t>
   </si>
   <si>
-    <t>Abu Bakr</t>
+    <t>NAME_HABIBA AFZAL ANSARI_MarkSheet_ency.pdf</t>
   </si>
   <si>
-    <t>Umar</t>
+    <t>NAME_INAAYA MOINUDDIN LUHAR_MarkSheet_ency.pdf</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -419,7 +419,7 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>